<commit_message>
data sets made by tutorial
</commit_message>
<xml_diff>
--- a/data sets/XLConnectExample2.xlsx
+++ b/data sets/XLConnectExample2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="8">
   <si>
     <t>weight</t>
   </si>
@@ -80,33 +80,465 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="true" applyFill="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="true">
-      <alignment wrapText="true"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyNumberFormat="true">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyFill="true" applyNumberFormat="true" borderId="0" fillId="3" fontId="0" numFmtId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf applyNumberFormat="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+  <cellXfs count="150">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="4"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Standard" xfId="0"/>
     <cellStyle name="XLConnect.Header" xfId="1"/>
     <cellStyle name="XLConnect.String" xfId="2"/>
     <cellStyle name="XLConnect.Numeric" xfId="3"/>
@@ -120,583 +552,583 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="true"/>
+    <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="1">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="3">
+      <c r="A2" s="8" t="n">
         <v>179.0</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="79" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="3">
+      <c r="A3" s="9" t="n">
         <v>160.0</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="80" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="3">
+      <c r="A4" s="10" t="n">
         <v>136.0</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="81" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n" s="3">
+      <c r="A5" s="11" t="n">
         <v>227.0</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="82" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n" s="3">
+      <c r="A6" s="12" t="n">
         <v>217.0</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="83" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n" s="3">
+      <c r="A7" s="13" t="n">
         <v>168.0</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="B7" s="84" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n" s="3">
+      <c r="A8" s="14" t="n">
         <v>108.0</v>
       </c>
-      <c r="B8" t="s" s="2">
+      <c r="B8" s="85" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n" s="3">
+      <c r="A9" s="15" t="n">
         <v>124.0</v>
       </c>
-      <c r="B9" t="s" s="2">
+      <c r="B9" s="86" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n" s="3">
+      <c r="A10" s="16" t="n">
         <v>143.0</v>
       </c>
-      <c r="B10" t="s" s="2">
+      <c r="B10" s="87" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n" s="3">
+      <c r="A11" s="17" t="n">
         <v>140.0</v>
       </c>
-      <c r="B11" t="s" s="2">
+      <c r="B11" s="88" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n" s="3">
+      <c r="A12" s="18" t="n">
         <v>309.0</v>
       </c>
-      <c r="B12" t="s" s="2">
+      <c r="B12" s="89" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n" s="3">
+      <c r="A13" s="19" t="n">
         <v>229.0</v>
       </c>
-      <c r="B13" t="s" s="2">
+      <c r="B13" s="90" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n" s="3">
+      <c r="A14" s="20" t="n">
         <v>181.0</v>
       </c>
-      <c r="B14" t="s" s="2">
+      <c r="B14" s="91" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="3">
+      <c r="A15" s="21" t="n">
         <v>141.0</v>
       </c>
-      <c r="B15" t="s" s="2">
+      <c r="B15" s="92" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="3">
+      <c r="A16" s="22" t="n">
         <v>260.0</v>
       </c>
-      <c r="B16" t="s" s="2">
+      <c r="B16" s="93" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n" s="3">
+      <c r="A17" s="23" t="n">
         <v>203.0</v>
       </c>
-      <c r="B17" t="s" s="2">
+      <c r="B17" s="94" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="n" s="3">
+      <c r="A18" s="24" t="n">
         <v>148.0</v>
       </c>
-      <c r="B18" t="s" s="2">
+      <c r="B18" s="95" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="n" s="3">
+      <c r="A19" s="25" t="n">
         <v>169.0</v>
       </c>
-      <c r="B19" t="s" s="2">
+      <c r="B19" s="96" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="n" s="3">
+      <c r="A20" s="26" t="n">
         <v>213.0</v>
       </c>
-      <c r="B20" t="s" s="2">
+      <c r="B20" s="97" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="n" s="3">
+      <c r="A21" s="27" t="n">
         <v>257.0</v>
       </c>
-      <c r="B21" t="s" s="2">
+      <c r="B21" s="98" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="n" s="3">
+      <c r="A22" s="28" t="n">
         <v>244.0</v>
       </c>
-      <c r="B22" t="s" s="2">
+      <c r="B22" s="99" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="n" s="3">
+      <c r="A23" s="29" t="n">
         <v>271.0</v>
       </c>
-      <c r="B23" t="s" s="2">
+      <c r="B23" s="100" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="n" s="3">
+      <c r="A24" s="30" t="n">
         <v>243.0</v>
       </c>
-      <c r="B24" t="s" s="2">
+      <c r="B24" s="101" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="n" s="3">
+      <c r="A25" s="31" t="n">
         <v>230.0</v>
       </c>
-      <c r="B25" t="s" s="2">
+      <c r="B25" s="102" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="n" s="3">
+      <c r="A26" s="32" t="n">
         <v>248.0</v>
       </c>
-      <c r="B26" t="s" s="2">
+      <c r="B26" s="103" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="n" s="3">
+      <c r="A27" s="33" t="n">
         <v>327.0</v>
       </c>
-      <c r="B27" t="s" s="2">
+      <c r="B27" s="104" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="n" s="3">
+      <c r="A28" s="34" t="n">
         <v>329.0</v>
       </c>
-      <c r="B28" t="s" s="2">
+      <c r="B28" s="105" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="n" s="3">
+      <c r="A29" s="35" t="n">
         <v>250.0</v>
       </c>
-      <c r="B29" t="s" s="2">
+      <c r="B29" s="106" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="n" s="3">
+      <c r="A30" s="36" t="n">
         <v>193.0</v>
       </c>
-      <c r="B30" t="s" s="2">
+      <c r="B30" s="107" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="n" s="3">
+      <c r="A31" s="37" t="n">
         <v>271.0</v>
       </c>
-      <c r="B31" t="s" s="2">
+      <c r="B31" s="108" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="n" s="3">
+      <c r="A32" s="38" t="n">
         <v>316.0</v>
       </c>
-      <c r="B32" t="s" s="2">
+      <c r="B32" s="109" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="n" s="3">
+      <c r="A33" s="39" t="n">
         <v>267.0</v>
       </c>
-      <c r="B33" t="s" s="2">
+      <c r="B33" s="110" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="n" s="3">
+      <c r="A34" s="40" t="n">
         <v>199.0</v>
       </c>
-      <c r="B34" t="s" s="2">
+      <c r="B34" s="111" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="n" s="3">
+      <c r="A35" s="41" t="n">
         <v>171.0</v>
       </c>
-      <c r="B35" t="s" s="2">
+      <c r="B35" s="112" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="n" s="3">
+      <c r="A36" s="42" t="n">
         <v>158.0</v>
       </c>
-      <c r="B36" t="s" s="2">
+      <c r="B36" s="113" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="n" s="3">
+      <c r="A37" s="43" t="n">
         <v>248.0</v>
       </c>
-      <c r="B37" t="s" s="2">
+      <c r="B37" s="114" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="n" s="3">
+      <c r="A38" s="44" t="n">
         <v>423.0</v>
       </c>
-      <c r="B38" t="s" s="2">
+      <c r="B38" s="115" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="n" s="3">
+      <c r="A39" s="45" t="n">
         <v>340.0</v>
       </c>
-      <c r="B39" t="s" s="2">
+      <c r="B39" s="116" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="n" s="3">
+      <c r="A40" s="46" t="n">
         <v>392.0</v>
       </c>
-      <c r="B40" t="s" s="2">
+      <c r="B40" s="117" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="n" s="3">
+      <c r="A41" s="47" t="n">
         <v>339.0</v>
       </c>
-      <c r="B41" t="s" s="2">
+      <c r="B41" s="118" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="n" s="3">
+      <c r="A42" s="48" t="n">
         <v>341.0</v>
       </c>
-      <c r="B42" t="s" s="2">
+      <c r="B42" s="119" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="n" s="3">
+      <c r="A43" s="49" t="n">
         <v>226.0</v>
       </c>
-      <c r="B43" t="s" s="2">
+      <c r="B43" s="120" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="n" s="3">
+      <c r="A44" s="50" t="n">
         <v>320.0</v>
       </c>
-      <c r="B44" t="s" s="2">
+      <c r="B44" s="121" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="n" s="3">
+      <c r="A45" s="51" t="n">
         <v>295.0</v>
       </c>
-      <c r="B45" t="s" s="2">
+      <c r="B45" s="122" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="n" s="3">
+      <c r="A46" s="52" t="n">
         <v>334.0</v>
       </c>
-      <c r="B46" t="s" s="2">
+      <c r="B46" s="123" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="n" s="3">
+      <c r="A47" s="53" t="n">
         <v>322.0</v>
       </c>
-      <c r="B47" t="s" s="2">
+      <c r="B47" s="124" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="n" s="3">
+      <c r="A48" s="54" t="n">
         <v>297.0</v>
       </c>
-      <c r="B48" t="s" s="2">
+      <c r="B48" s="125" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="n" s="3">
+      <c r="A49" s="55" t="n">
         <v>318.0</v>
       </c>
-      <c r="B49" t="s" s="2">
+      <c r="B49" s="126" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="n" s="3">
+      <c r="A50" s="56" t="n">
         <v>325.0</v>
       </c>
-      <c r="B50" t="s" s="2">
+      <c r="B50" s="127" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="n" s="3">
+      <c r="A51" s="57" t="n">
         <v>257.0</v>
       </c>
-      <c r="B51" t="s" s="2">
+      <c r="B51" s="128" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="n" s="3">
+      <c r="A52" s="58" t="n">
         <v>303.0</v>
       </c>
-      <c r="B52" t="s" s="2">
+      <c r="B52" s="129" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="n" s="3">
+      <c r="A53" s="59" t="n">
         <v>315.0</v>
       </c>
-      <c r="B53" t="s" s="2">
+      <c r="B53" s="130" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="n" s="3">
+      <c r="A54" s="60" t="n">
         <v>380.0</v>
       </c>
-      <c r="B54" t="s" s="2">
+      <c r="B54" s="131" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="n" s="3">
+      <c r="A55" s="61" t="n">
         <v>153.0</v>
       </c>
-      <c r="B55" t="s" s="2">
+      <c r="B55" s="132" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="n" s="3">
+      <c r="A56" s="62" t="n">
         <v>263.0</v>
       </c>
-      <c r="B56" t="s" s="2">
+      <c r="B56" s="133" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="n" s="3">
+      <c r="A57" s="63" t="n">
         <v>242.0</v>
       </c>
-      <c r="B57" t="s" s="2">
+      <c r="B57" s="134" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="n" s="3">
+      <c r="A58" s="64" t="n">
         <v>206.0</v>
       </c>
-      <c r="B58" t="s" s="2">
+      <c r="B58" s="135" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="n" s="3">
+      <c r="A59" s="65" t="n">
         <v>344.0</v>
       </c>
-      <c r="B59" t="s" s="2">
+      <c r="B59" s="136" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="n" s="3">
+      <c r="A60" s="66" t="n">
         <v>258.0</v>
       </c>
-      <c r="B60" t="s" s="2">
+      <c r="B60" s="137" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="n" s="3">
+      <c r="A61" s="67" t="n">
         <v>368.0</v>
       </c>
-      <c r="B61" t="s" s="2">
+      <c r="B61" s="138" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="n" s="3">
+      <c r="A62" s="68" t="n">
         <v>390.0</v>
       </c>
-      <c r="B62" t="s" s="2">
+      <c r="B62" s="139" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="n" s="3">
+      <c r="A63" s="69" t="n">
         <v>379.0</v>
       </c>
-      <c r="B63" t="s" s="2">
+      <c r="B63" s="140" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="n" s="3">
+      <c r="A64" s="70" t="n">
         <v>260.0</v>
       </c>
-      <c r="B64" t="s" s="2">
+      <c r="B64" s="141" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="n" s="3">
+      <c r="A65" s="71" t="n">
         <v>404.0</v>
       </c>
-      <c r="B65" t="s" s="2">
+      <c r="B65" s="142" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="n" s="3">
+      <c r="A66" s="72" t="n">
         <v>318.0</v>
       </c>
-      <c r="B66" t="s" s="2">
+      <c r="B66" s="143" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="n" s="3">
+      <c r="A67" s="73" t="n">
         <v>352.0</v>
       </c>
-      <c r="B67" t="s" s="2">
+      <c r="B67" s="144" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="n" s="3">
+      <c r="A68" s="74" t="n">
         <v>359.0</v>
       </c>
-      <c r="B68" t="s" s="2">
+      <c r="B68" s="145" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="n" s="3">
+      <c r="A69" s="75" t="n">
         <v>216.0</v>
       </c>
-      <c r="B69" t="s" s="2">
+      <c r="B69" s="146" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="n" s="3">
+      <c r="A70" s="76" t="n">
         <v>222.0</v>
       </c>
-      <c r="B70" t="s" s="2">
+      <c r="B70" s="147" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="n" s="3">
+      <c r="A71" s="77" t="n">
         <v>283.0</v>
       </c>
-      <c r="B71" t="s" s="2">
+      <c r="B71" s="148" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="n" s="3">
+      <c r="A72" s="78" t="n">
         <v>332.0</v>
       </c>
-      <c r="B72" t="s" s="2">
+      <c r="B72" s="149" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
datasets due to practicing
</commit_message>
<xml_diff>
--- a/data sets/XLConnectExample2.xlsx
+++ b/data sets/XLConnectExample2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="8">
   <si>
     <t>weight</t>
   </si>
@@ -97,13 +97,445 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="294">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="4"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="5"/>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="1">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="3">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="1">
       <alignment wrapText="true"/>
     </xf>
@@ -557,578 +989,578 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="150" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="151" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="n">
+      <c r="A2" s="152" t="n">
         <v>179.0</v>
       </c>
-      <c r="B2" s="79" t="s">
+      <c r="B2" s="223" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9" t="n">
+      <c r="A3" s="153" t="n">
         <v>160.0</v>
       </c>
-      <c r="B3" s="80" t="s">
+      <c r="B3" s="224" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="10" t="n">
+      <c r="A4" s="154" t="n">
         <v>136.0</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="225" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="11" t="n">
+      <c r="A5" s="155" t="n">
         <v>227.0</v>
       </c>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="226" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="12" t="n">
+      <c r="A6" s="156" t="n">
         <v>217.0</v>
       </c>
-      <c r="B6" s="83" t="s">
+      <c r="B6" s="227" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="n">
+      <c r="A7" s="157" t="n">
         <v>168.0</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="228" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="14" t="n">
+      <c r="A8" s="158" t="n">
         <v>108.0</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="229" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="15" t="n">
+      <c r="A9" s="159" t="n">
         <v>124.0</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="230" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="16" t="n">
+      <c r="A10" s="160" t="n">
         <v>143.0</v>
       </c>
-      <c r="B10" s="87" t="s">
+      <c r="B10" s="231" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="17" t="n">
+      <c r="A11" s="161" t="n">
         <v>140.0</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="232" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="18" t="n">
+      <c r="A12" s="162" t="n">
         <v>309.0</v>
       </c>
-      <c r="B12" s="89" t="s">
+      <c r="B12" s="233" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="19" t="n">
+      <c r="A13" s="163" t="n">
         <v>229.0</v>
       </c>
-      <c r="B13" s="90" t="s">
+      <c r="B13" s="234" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="20" t="n">
+      <c r="A14" s="164" t="n">
         <v>181.0</v>
       </c>
-      <c r="B14" s="91" t="s">
+      <c r="B14" s="235" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="21" t="n">
+      <c r="A15" s="165" t="n">
         <v>141.0</v>
       </c>
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="236" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="22" t="n">
+      <c r="A16" s="166" t="n">
         <v>260.0</v>
       </c>
-      <c r="B16" s="93" t="s">
+      <c r="B16" s="237" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="23" t="n">
+      <c r="A17" s="167" t="n">
         <v>203.0</v>
       </c>
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="238" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="24" t="n">
+      <c r="A18" s="168" t="n">
         <v>148.0</v>
       </c>
-      <c r="B18" s="95" t="s">
+      <c r="B18" s="239" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="25" t="n">
+      <c r="A19" s="169" t="n">
         <v>169.0</v>
       </c>
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="240" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="26" t="n">
+      <c r="A20" s="170" t="n">
         <v>213.0</v>
       </c>
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="241" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="n">
+      <c r="A21" s="171" t="n">
         <v>257.0</v>
       </c>
-      <c r="B21" s="98" t="s">
+      <c r="B21" s="242" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="28" t="n">
+      <c r="A22" s="172" t="n">
         <v>244.0</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="243" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="29" t="n">
+      <c r="A23" s="173" t="n">
         <v>271.0</v>
       </c>
-      <c r="B23" s="100" t="s">
+      <c r="B23" s="244" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="30" t="n">
+      <c r="A24" s="174" t="n">
         <v>243.0</v>
       </c>
-      <c r="B24" s="101" t="s">
+      <c r="B24" s="245" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="31" t="n">
+      <c r="A25" s="175" t="n">
         <v>230.0</v>
       </c>
-      <c r="B25" s="102" t="s">
+      <c r="B25" s="246" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="32" t="n">
+      <c r="A26" s="176" t="n">
         <v>248.0</v>
       </c>
-      <c r="B26" s="103" t="s">
+      <c r="B26" s="247" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="33" t="n">
+      <c r="A27" s="177" t="n">
         <v>327.0</v>
       </c>
-      <c r="B27" s="104" t="s">
+      <c r="B27" s="248" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="34" t="n">
+      <c r="A28" s="178" t="n">
         <v>329.0</v>
       </c>
-      <c r="B28" s="105" t="s">
+      <c r="B28" s="249" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="35" t="n">
+      <c r="A29" s="179" t="n">
         <v>250.0</v>
       </c>
-      <c r="B29" s="106" t="s">
+      <c r="B29" s="250" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="36" t="n">
+      <c r="A30" s="180" t="n">
         <v>193.0</v>
       </c>
-      <c r="B30" s="107" t="s">
+      <c r="B30" s="251" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="37" t="n">
+      <c r="A31" s="181" t="n">
         <v>271.0</v>
       </c>
-      <c r="B31" s="108" t="s">
+      <c r="B31" s="252" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="38" t="n">
+      <c r="A32" s="182" t="n">
         <v>316.0</v>
       </c>
-      <c r="B32" s="109" t="s">
+      <c r="B32" s="253" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="39" t="n">
+      <c r="A33" s="183" t="n">
         <v>267.0</v>
       </c>
-      <c r="B33" s="110" t="s">
+      <c r="B33" s="254" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="40" t="n">
+      <c r="A34" s="184" t="n">
         <v>199.0</v>
       </c>
-      <c r="B34" s="111" t="s">
+      <c r="B34" s="255" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="41" t="n">
+      <c r="A35" s="185" t="n">
         <v>171.0</v>
       </c>
-      <c r="B35" s="112" t="s">
+      <c r="B35" s="256" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="42" t="n">
+      <c r="A36" s="186" t="n">
         <v>158.0</v>
       </c>
-      <c r="B36" s="113" t="s">
+      <c r="B36" s="257" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="43" t="n">
+      <c r="A37" s="187" t="n">
         <v>248.0</v>
       </c>
-      <c r="B37" s="114" t="s">
+      <c r="B37" s="258" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="44" t="n">
+      <c r="A38" s="188" t="n">
         <v>423.0</v>
       </c>
-      <c r="B38" s="115" t="s">
+      <c r="B38" s="259" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="45" t="n">
+      <c r="A39" s="189" t="n">
         <v>340.0</v>
       </c>
-      <c r="B39" s="116" t="s">
+      <c r="B39" s="260" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="46" t="n">
+      <c r="A40" s="190" t="n">
         <v>392.0</v>
       </c>
-      <c r="B40" s="117" t="s">
+      <c r="B40" s="261" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="47" t="n">
+      <c r="A41" s="191" t="n">
         <v>339.0</v>
       </c>
-      <c r="B41" s="118" t="s">
+      <c r="B41" s="262" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="48" t="n">
+      <c r="A42" s="192" t="n">
         <v>341.0</v>
       </c>
-      <c r="B42" s="119" t="s">
+      <c r="B42" s="263" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="49" t="n">
+      <c r="A43" s="193" t="n">
         <v>226.0</v>
       </c>
-      <c r="B43" s="120" t="s">
+      <c r="B43" s="264" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="50" t="n">
+      <c r="A44" s="194" t="n">
         <v>320.0</v>
       </c>
-      <c r="B44" s="121" t="s">
+      <c r="B44" s="265" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="51" t="n">
+      <c r="A45" s="195" t="n">
         <v>295.0</v>
       </c>
-      <c r="B45" s="122" t="s">
+      <c r="B45" s="266" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="52" t="n">
+      <c r="A46" s="196" t="n">
         <v>334.0</v>
       </c>
-      <c r="B46" s="123" t="s">
+      <c r="B46" s="267" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="53" t="n">
+      <c r="A47" s="197" t="n">
         <v>322.0</v>
       </c>
-      <c r="B47" s="124" t="s">
+      <c r="B47" s="268" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="54" t="n">
+      <c r="A48" s="198" t="n">
         <v>297.0</v>
       </c>
-      <c r="B48" s="125" t="s">
+      <c r="B48" s="269" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="55" t="n">
+      <c r="A49" s="199" t="n">
         <v>318.0</v>
       </c>
-      <c r="B49" s="126" t="s">
+      <c r="B49" s="270" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="56" t="n">
+      <c r="A50" s="200" t="n">
         <v>325.0</v>
       </c>
-      <c r="B50" s="127" t="s">
+      <c r="B50" s="271" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="57" t="n">
+      <c r="A51" s="201" t="n">
         <v>257.0</v>
       </c>
-      <c r="B51" s="128" t="s">
+      <c r="B51" s="272" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="58" t="n">
+      <c r="A52" s="202" t="n">
         <v>303.0</v>
       </c>
-      <c r="B52" s="129" t="s">
+      <c r="B52" s="273" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="59" t="n">
+      <c r="A53" s="203" t="n">
         <v>315.0</v>
       </c>
-      <c r="B53" s="130" t="s">
+      <c r="B53" s="274" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="60" t="n">
+      <c r="A54" s="204" t="n">
         <v>380.0</v>
       </c>
-      <c r="B54" s="131" t="s">
+      <c r="B54" s="275" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="61" t="n">
+      <c r="A55" s="205" t="n">
         <v>153.0</v>
       </c>
-      <c r="B55" s="132" t="s">
+      <c r="B55" s="276" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="62" t="n">
+      <c r="A56" s="206" t="n">
         <v>263.0</v>
       </c>
-      <c r="B56" s="133" t="s">
+      <c r="B56" s="277" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="63" t="n">
+      <c r="A57" s="207" t="n">
         <v>242.0</v>
       </c>
-      <c r="B57" s="134" t="s">
+      <c r="B57" s="278" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="64" t="n">
+      <c r="A58" s="208" t="n">
         <v>206.0</v>
       </c>
-      <c r="B58" s="135" t="s">
+      <c r="B58" s="279" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="65" t="n">
+      <c r="A59" s="209" t="n">
         <v>344.0</v>
       </c>
-      <c r="B59" s="136" t="s">
+      <c r="B59" s="280" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="66" t="n">
+      <c r="A60" s="210" t="n">
         <v>258.0</v>
       </c>
-      <c r="B60" s="137" t="s">
+      <c r="B60" s="281" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="67" t="n">
+      <c r="A61" s="211" t="n">
         <v>368.0</v>
       </c>
-      <c r="B61" s="138" t="s">
+      <c r="B61" s="282" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="68" t="n">
+      <c r="A62" s="212" t="n">
         <v>390.0</v>
       </c>
-      <c r="B62" s="139" t="s">
+      <c r="B62" s="283" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="69" t="n">
+      <c r="A63" s="213" t="n">
         <v>379.0</v>
       </c>
-      <c r="B63" s="140" t="s">
+      <c r="B63" s="284" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="70" t="n">
+      <c r="A64" s="214" t="n">
         <v>260.0</v>
       </c>
-      <c r="B64" s="141" t="s">
+      <c r="B64" s="285" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="71" t="n">
+      <c r="A65" s="215" t="n">
         <v>404.0</v>
       </c>
-      <c r="B65" s="142" t="s">
+      <c r="B65" s="286" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="72" t="n">
+      <c r="A66" s="216" t="n">
         <v>318.0</v>
       </c>
-      <c r="B66" s="143" t="s">
+      <c r="B66" s="287" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="73" t="n">
+      <c r="A67" s="217" t="n">
         <v>352.0</v>
       </c>
-      <c r="B67" s="144" t="s">
+      <c r="B67" s="288" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="74" t="n">
+      <c r="A68" s="218" t="n">
         <v>359.0</v>
       </c>
-      <c r="B68" s="145" t="s">
+      <c r="B68" s="289" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="75" t="n">
+      <c r="A69" s="219" t="n">
         <v>216.0</v>
       </c>
-      <c r="B69" s="146" t="s">
+      <c r="B69" s="290" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="76" t="n">
+      <c r="A70" s="220" t="n">
         <v>222.0</v>
       </c>
-      <c r="B70" s="147" t="s">
+      <c r="B70" s="291" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="77" t="n">
+      <c r="A71" s="221" t="n">
         <v>283.0</v>
       </c>
-      <c r="B71" s="148" t="s">
+      <c r="B71" s="292" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="78" t="n">
+      <c r="A72" s="222" t="n">
         <v>332.0</v>
       </c>
-      <c r="B72" s="149" t="s">
+      <c r="B72" s="293" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>